<commit_message>
Updated paper.  Sent draft to Eric and Ali
</commit_message>
<xml_diff>
--- a/docs/csRPE-tkloData.xlsx
+++ b/docs/csRPE-tkloData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22140" activeTab="1"/>
+    <workbookView xWindow="980" yWindow="400" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="projects" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>URL</t>
   </si>
@@ -141,13 +141,28 @@
   </si>
   <si>
     <t>Iteration 1</t>
+  </si>
+  <si>
+    <t>RevealJS</t>
+  </si>
+  <si>
+    <t>https://github.com/hakimel/reveal.js/tree/master/test</t>
+  </si>
+  <si>
+    <t>Qunit</t>
+  </si>
+  <si>
+    <t>http://todomvc.com/</t>
+  </si>
+  <si>
+    <t>CodeAcademy, Code School, Code, TreeHouse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +174,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,11 +204,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -198,13 +223,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -505,16 +538,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="5" width="12.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="34.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="53" style="2" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" style="2"/>
     <col min="8" max="8" width="22.5" style="2" customWidth="1"/>
     <col min="9" max="9" width="29.83203125" style="2" customWidth="1"/>
@@ -720,12 +753,43 @@
         <v>12</v>
       </c>
     </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6">
+      <c r="F17" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6">
+      <c r="F23" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F13" r:id="rId1"/>
     <hyperlink ref="F6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -738,7 +802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -748,11 +812,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" s="2" t="s">
@@ -766,7 +830,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="2">

</xml_diff>